<commit_message>
CHG : EnemyDataTable 구조 변경
</commit_message>
<xml_diff>
--- a/DataTables/DT_MonsterStaticData.xlsx
+++ b/DataTables/DT_MonsterStaticData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Potenup_3rd\Project\MageSquad\DataTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\Project\MageSquad\DataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9F455C-70D4-40AA-A91D-20471AC917E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5007FA6B-F527-467E-8DCC-0EB402EC20F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="465" yWindow="2265" windowWidth="33420" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MonsterStaticData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>SkeletalMesh</t>
   </si>
@@ -53,12 +53,6 @@
     <t>AttackRange</t>
   </si>
   <si>
-    <t>StartAbilities</t>
-  </si>
-  <si>
-    <t>StartEffects</t>
-  </si>
-  <si>
     <t>bIsRanged</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
     <t>/Game/Data/Enemy/DA/Normal/DA_GhoulAnimData.DA_GhoulAnimData</t>
   </si>
   <si>
-    <t>(/Game/Blueprints/GAS/GA/Enemy/BPGA_EnemyNormalAttack.BPGA_EnemyNormalAttack_C,/Game/Blueprints/GAS/GA/Enemy/BPGA_EnemyDead.BPGA_EnemyDead_C,/Game/Blueprints/GAS/GA/Shared/BPGA_DamageFloater.BPGA_DamageFloater_C)</t>
-  </si>
-  <si>
     <t>Normal_Lich</t>
   </si>
   <si>
@@ -120,18 +111,10 @@
     <t>/Game/Data/Enemy/DA/Boss/DA_SevarogAnimData.DA_SevarogAnimData</t>
   </si>
   <si>
-    <t>(/Game/Blueprints/GAS/GA/Enemy/BPGA_EnemyNormalAttack.BPGA_EnemyNormalAttack_C,/Game/Blueprints/GAS/GA/Enemy/BPGA_EnemyDead.BPGA_EnemyDead_C,/Game/Blueprints/GAS/GA/Shared/BPGA_DamageFloater.BPGA_DamageFloater_C, /Game/Blueprints/GAS/GA/Enemy/BPGA_EnemySpawn.BPGA_EnemySpawn_C)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>DropExpValue</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/Game/Aseets/ParagonSevarog/Characters/Heroes/Sevarog/Skins/Tier_1/Sevarog_Chronos/Meshes/SevarogChronos.SevarogChronos</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Boss_Fey</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -148,7 +131,23 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/Game/Blueprints/GAS/GA/Player/Passive/IceSpear/BP_IceSpearProjectile.BP_IceSpearProjectile_C</t>
+    <t>/Game/Data/Enemy/DA/Normal/DA_NormalEnemyAbilitiesData.DA_NormalEnemyAbilitiesData</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Game/Data/Enemy/DA/Boss/DA_BossEnemyAbilitiesData.DA_BossEnemyAbilitiesData</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Game/Personal/LIM_H_S/BP_LichAttack.BP_LichAttack_C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Game/Aseets/ParagonSevarog/Characters/Heroes/Sevarog/Meshes/Sevarog.Sevarog</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnemyAbilities</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -548,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -562,13 +561,15 @@
     <col min="4" max="5" width="12" customWidth="1"/>
     <col min="6" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="60" customWidth="1"/>
-    <col min="9" max="9" width="40" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="16.125" customWidth="1"/>
+    <col min="11" max="11" width="23.5" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -589,30 +590,27 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="2">
         <v>80</v>
@@ -627,25 +625,24 @@
         <v>150</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="b">
+        <v>30</v>
+      </c>
+      <c r="I2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="K2" s="3">
+      <c r="J2" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2">
         <v>100</v>
@@ -660,28 +657,27 @@
         <v>1000</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3">
+        <v>15</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2">
         <v>70</v>
@@ -696,25 +692,24 @@
         <v>150</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2" t="b">
+        <v>30</v>
+      </c>
+      <c r="I4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="K4" s="3">
+      <c r="J4" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2">
         <v>50</v>
@@ -729,25 +724,24 @@
         <v>150</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2" t="b">
+        <v>30</v>
+      </c>
+      <c r="I5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="K5" s="3">
+      <c r="J5" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2">
         <v>60</v>
@@ -762,25 +756,24 @@
         <v>150</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2" t="b">
+        <v>30</v>
+      </c>
+      <c r="I6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="K6" s="3">
+      <c r="J6" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D7" s="4">
         <v>50000</v>
@@ -795,22 +788,21 @@
         <v>1500</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="D8" s="4">
         <v>50000</v>
@@ -825,13 +817,12 @@
         <v>1500</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4" t="b">
+        <v>31</v>
+      </c>
+      <c r="I8" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="K8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
NEW : Phase2가 되면 SkeletalMesh가 변경되는 기능 추가
</commit_message>
<xml_diff>
--- a/DataTables/DT_MonsterStaticData.xlsx
+++ b/DataTables/DT_MonsterStaticData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\Project\MageSquad\DataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5007FA6B-F527-467E-8DCC-0EB402EC20F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F498E66D-D12C-4EFB-8219-0C847BA0B39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="465" yWindow="2265" windowWidth="33420" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>SkeletalMesh</t>
   </si>
@@ -148,6 +148,14 @@
   </si>
   <si>
     <t>EnemyAbilities</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phase2SkeletalMesh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Game/Aseets/ParagonSevarog/Characters/Heroes/Sevarog/Skins/Tier_1_5/MaskedReaper/Mesh/Sevarog_MaskedReaper_GDC.Sevarog_MaskedReaper_GDC</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -205,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -228,11 +236,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,6 +279,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -547,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -564,10 +605,10 @@
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="16.125" customWidth="1"/>
     <col min="11" max="11" width="23.5" customWidth="1"/>
-    <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="12" max="12" width="28.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -598,11 +639,14 @@
       <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="10" t="s">
         <v>29</v>
       </c>
+      <c r="L1" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -622,7 +666,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="2">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>30</v>
@@ -630,11 +674,12 @@
       <c r="I2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="6">
         <v>10</v>
       </c>
+      <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -662,14 +707,15 @@
       <c r="I3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="6">
         <v>15</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -689,7 +735,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="2">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>30</v>
@@ -697,11 +743,12 @@
       <c r="I4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="6">
         <v>10</v>
       </c>
+      <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -721,7 +768,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="2">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>30</v>
@@ -729,11 +776,12 @@
       <c r="I5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="6">
         <v>20</v>
       </c>
+      <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -753,7 +801,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="2">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>30</v>
@@ -761,11 +809,12 @@
       <c r="I6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="6">
         <v>20</v>
       </c>
+      <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -793,8 +842,13 @@
       <c r="I7" s="4" t="b">
         <v>1</v>
       </c>
+      <c r="J7" s="7"/>
+      <c r="L7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
NEW : 보스 DirectionIndicator 추가
</commit_message>
<xml_diff>
--- a/DataTables/DT_MonsterStaticData.xlsx
+++ b/DataTables/DT_MonsterStaticData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Potenup_3rd\Project\MageSquad\DataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFDD77D-BDD1-4A12-944E-524EBC203E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3783D06-C928-44E3-887B-C314D2E16248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="345" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MonsterStaticData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>SkeletalMesh</t>
   </si>
@@ -115,18 +115,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Boss_Fey</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Game/Aseets/ParagonFey/Characters/Heroes/Fey/Meshes/Fey_GDC.Fey_GDC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Game/Data/Enemy/DA/Boss/DA_FeyAnimData.DA_FeyAnimData</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>ProjectileDataClass</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -168,6 +156,37 @@
   </si>
   <si>
     <t>/Game/Data/Enemy/DA/Normal/DA_BatAnimData.DA_BatAnimData</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Ind</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>catorImage</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Game/Sprites/T_BossImage.T_BossImage</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -175,7 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,8 +217,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +247,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -294,10 +326,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -602,22 +640,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="57.25" customWidth="1"/>
-    <col min="3" max="3" width="73.5" customWidth="1"/>
-    <col min="4" max="5" width="12" customWidth="1"/>
-    <col min="6" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="60" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="16.125" customWidth="1"/>
-    <col min="11" max="11" width="23.5" customWidth="1"/>
-    <col min="12" max="12" width="28.625" customWidth="1"/>
+    <col min="1" max="1" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="89.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="147" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="63.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -643,7 +684,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -651,11 +692,14 @@
       <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>35</v>
+      <c r="K1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -681,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I2" s="2" t="b">
         <v>0</v>
@@ -714,7 +758,7 @@
         <v>1000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I3" s="2" t="b">
         <v>1</v>
@@ -723,7 +767,7 @@
         <v>15</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M3" s="8"/>
     </row>
@@ -750,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I4" s="2" t="b">
         <v>0</v>
@@ -783,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I5" s="2" t="b">
         <v>0</v>
@@ -795,13 +839,13 @@
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2">
         <v>100</v>
@@ -816,7 +860,7 @@
         <v>700</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I6" s="2" t="b">
         <v>1</v>
@@ -825,7 +869,7 @@
         <v>20</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M6" s="8"/>
     </row>
@@ -852,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I7" s="2" t="b">
         <v>0</v>
@@ -867,13 +911,13 @@
         <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="4">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E8" s="4">
         <v>400</v>
@@ -882,49 +926,33 @@
         <v>50</v>
       </c>
       <c r="G8" s="4">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I8" s="4" t="b">
         <v>1</v>
       </c>
       <c r="J8" s="7"/>
       <c r="L8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M8" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="4">
-        <v>50000</v>
-      </c>
-      <c r="E9" s="4">
-        <v>400</v>
-      </c>
-      <c r="F9" s="4">
-        <v>50</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1500</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" s="5"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
NEW : Elite Enemy 제작
</commit_message>
<xml_diff>
--- a/DataTables/DT_MonsterStaticData.xlsx
+++ b/DataTables/DT_MonsterStaticData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Potenup_3rd\Project\MageSquad\DataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3783D06-C928-44E3-887B-C314D2E16248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E515723-C35E-49DA-8C5C-740B3BE317D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>SkeletalMesh</t>
   </si>
@@ -187,6 +187,30 @@
   </si>
   <si>
     <t>/Game/Sprites/T_BossImage.T_BossImage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elite_Ghoul</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elite_Lich</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elite_Spider</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elite_Goblin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elite_Bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elite_Toad</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -252,7 +276,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -329,13 +353,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -638,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -698,7 +721,7 @@
       <c r="L1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
@@ -907,52 +930,267 @@
       <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="10">
+        <f>D2*5</f>
+        <v>400</v>
+      </c>
+      <c r="E8" s="10">
+        <v>300</v>
+      </c>
+      <c r="F8" s="10">
+        <f>F2*2</f>
+        <v>30</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
+        <v>10</v>
+      </c>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="13"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="10">
+        <f>D3*5</f>
+        <v>500</v>
+      </c>
+      <c r="E9" s="10">
+        <v>350</v>
+      </c>
+      <c r="F9" s="10">
+        <f>F3*2</f>
+        <v>40</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1000</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="11">
+        <v>15</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="12"/>
+      <c r="M9" s="13"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="10">
+        <f>D4*5</f>
+        <v>350</v>
+      </c>
+      <c r="E10" s="10">
+        <v>350</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" ref="F10:F13" si="0">F4*2</f>
+        <v>30</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11">
+        <v>10</v>
+      </c>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="13"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="10">
+        <f>D5*5</f>
+        <v>250</v>
+      </c>
+      <c r="E11" s="10">
+        <v>400</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="11">
+        <v>20</v>
+      </c>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="13"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="10">
+        <f>D6*5</f>
+        <v>500</v>
+      </c>
+      <c r="E12" s="10">
+        <v>350</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G12" s="10">
+        <v>700</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="11">
+        <v>20</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12" s="12"/>
+      <c r="M12" s="13"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="10">
+        <f>D7*5</f>
+        <v>300</v>
+      </c>
+      <c r="E13" s="10">
+        <v>330</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="11">
+        <v>20</v>
+      </c>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="13"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D14" s="4">
         <v>1000</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E14" s="4">
         <v>400</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F14" s="4">
         <v>50</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G14" s="4">
         <v>1000</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="4" t="b">
+      <c r="I14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="L8" s="5" t="s">
+      <c r="J14" s="7"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M14" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>